<commit_message>
Changes of 28th July 2022
</commit_message>
<xml_diff>
--- a/Connect/src/main/resources/connect_TestData/OrderCreation.xlsx
+++ b/Connect/src/main/resources/connect_TestData/OrderCreation.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="171">
   <si>
     <t>Abhishek</t>
   </si>
@@ -1124,7 +1124,7 @@
         <v>77</v>
       </c>
       <c r="AB2" t="s">
-        <v>77</v>
+        <v>128</v>
       </c>
       <c r="AC2" s="1" t="s">
         <v>72</v>

</xml_diff>

<commit_message>
Changes of 2nd Aug 2022
</commit_message>
<xml_diff>
--- a/Connect/src/main/resources/connect_TestData/OrderCreation.xlsx
+++ b/Connect/src/main/resources/connect_TestData/OrderCreation.xlsx
@@ -4,18 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="570" windowWidth="7995" windowHeight="7725" tabRatio="614"/>
+    <workbookView tabRatio="614" windowHeight="7725" windowWidth="7995" xWindow="390" yWindow="570"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
-    <sheet name="SPL" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" r:id="rId1" sheetId="2"/>
+    <sheet name="SPL" r:id="rId2" sheetId="3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="176">
   <si>
     <t>Abhishek</t>
   </si>
@@ -478,12 +478,79 @@
   </si>
   <si>
     <t>RVOza</t>
+  </si>
+  <si>
+    <t>3482116</t>
+  </si>
+  <si>
+    <t>1127</t>
+  </si>
+  <si>
+    <t>1104</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>1105</t>
+  </si>
+  <si>
+    <t>3486248</t>
+  </si>
+  <si>
+    <t>1102</t>
+  </si>
+  <si>
+    <t>3486293</t>
+  </si>
+  <si>
+    <t>3486296</t>
+  </si>
+  <si>
+    <t>3486297</t>
+  </si>
+  <si>
+    <t>3486337</t>
+  </si>
+  <si>
+    <t>3486339</t>
+  </si>
+  <si>
+    <t>3486340</t>
+  </si>
+  <si>
+    <t>3486342</t>
+  </si>
+  <si>
+    <t>3486345</t>
+  </si>
+  <si>
+    <t>3486346</t>
+  </si>
+  <si>
+    <t>3486349</t>
+  </si>
+  <si>
+    <t>3486351</t>
+  </si>
+  <si>
+    <t>3486352</t>
+  </si>
+  <si>
+    <t>3486375</t>
+  </si>
+  <si>
+    <t>3486389</t>
+  </si>
+  <si>
+    <t>3486395</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -546,50 +613,50 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="17">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="1" numFmtId="49" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="1" numFmtId="49" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="2" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="3" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="1" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="1" numFmtId="49" quotePrefix="1" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -603,10 +670,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -764,7 +831,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -773,13 +840,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -789,7 +856,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -798,7 +865,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -807,7 +874,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -817,12 +884,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -853,7 +920,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -872,7 +939,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -884,8 +951,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AI11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
@@ -893,44 +960,44 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="20.7109375" style="3" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.28515625" style="3" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.42578125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.5703125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.85546875" style="3" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="9.28515625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="17.85546875" style="3" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="17.28515625" style="3" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="8.42578125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="17.28515625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="21.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="12.140625" style="3" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="8" style="3" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="11" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="10.140625" style="3" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="10.42578125" style="3" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="9.85546875" style="3" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="7.5703125" style="3" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="12.140625" style="3" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="9.7109375" style="3" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="17.28515625" style="3" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="13.5703125" style="3" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="13.28515625" style="3" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="13.140625" style="3" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="12.7109375" style="3" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="16.140625" style="3" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="17.5703125" style="3" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="18.140625" style="4" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="14.28515625" style="3" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="18.140625" style="3" customWidth="1" collapsed="1"/>
-    <col min="35" max="16384" width="9.140625" style="8" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="19.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="3" width="20.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="3" width="18.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="3" width="8.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="3" width="19.7109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="3" width="19.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="3" width="13.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="3" width="9.28515625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="3" width="13.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="3" width="17.85546875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="3" width="17.28515625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="3" width="8.42578125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="3" width="17.28515625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="3" width="21.7109375" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" style="3" width="12.140625" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" style="3" width="8.0" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="3" width="11.0" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" style="3" width="10.140625" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" style="3" width="10.42578125" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" style="3" width="9.85546875" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" style="3" width="7.5703125" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" style="3" width="12.140625" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" style="3" width="9.7109375" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" style="3" width="17.28515625" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" style="3" width="13.5703125" collapsed="true"/>
+    <col min="26" max="26" customWidth="true" style="3" width="13.28515625" collapsed="true"/>
+    <col min="27" max="27" customWidth="true" style="3" width="13.140625" collapsed="true"/>
+    <col min="28" max="28" customWidth="true" style="3" width="12.7109375" collapsed="true"/>
+    <col min="29" max="29" customWidth="true" style="3" width="16.140625" collapsed="true"/>
+    <col min="30" max="30" customWidth="true" style="3" width="17.5703125" collapsed="true"/>
+    <col min="31" max="31" customWidth="true" style="4" width="18.140625" collapsed="true"/>
+    <col min="32" max="32" customWidth="true" style="3" width="14.28515625" collapsed="true"/>
+    <col min="33" max="33" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="34" max="34" customWidth="true" style="3" width="18.140625" collapsed="true"/>
+    <col min="35" max="16384" style="8" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="25.5">
+    <row ht="25.5" r="1" spans="1:34">
       <c r="A1" s="10" t="s">
         <v>7</v>
       </c>
@@ -1032,7 +1099,7 @@
       </c>
       <c r="AH1" s="12"/>
     </row>
-    <row r="2" spans="1:34" ht="38.25">
+    <row ht="38.25" r="2" spans="1:34">
       <c r="A2" s="13" t="s">
         <v>10</v>
       </c>
@@ -1100,33 +1167,33 @@
       <c r="Y2" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="Z2" s="16" t="s">
+      <c r="Z2" t="s">
         <v>72</v>
       </c>
       <c r="AA2" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="AB2" s="16" t="s">
-        <v>127</v>
+      <c r="AB2" t="s">
+        <v>68</v>
       </c>
       <c r="AC2" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="AD2" s="16" t="s">
-        <v>70</v>
+      <c r="AD2" t="s">
+        <v>97</v>
       </c>
       <c r="AE2" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="AF2" s="16" t="s">
+      <c r="AF2" t="s">
         <v>127</v>
       </c>
-      <c r="AG2" s="16" t="s">
-        <v>148</v>
+      <c r="AG2" t="s">
+        <v>175</v>
       </c>
       <c r="AH2" s="15"/>
     </row>
-    <row r="3" spans="1:34" ht="51">
+    <row ht="51" r="3" spans="1:34">
       <c r="A3" s="13" t="s">
         <v>10</v>
       </c>
@@ -1198,20 +1265,20 @@
       <c r="Y3" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="Z3" s="16" t="s">
-        <v>73</v>
+      <c r="Z3" t="s">
+        <v>144</v>
       </c>
       <c r="AA3" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="AB3" s="16" t="s">
-        <v>75</v>
+      <c r="AB3" t="s">
+        <v>68</v>
       </c>
       <c r="AC3" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="AD3" s="16" t="s">
-        <v>77</v>
+      <c r="AD3" t="s">
+        <v>97</v>
       </c>
       <c r="AE3" s="13"/>
       <c r="AF3" s="16" t="s">
@@ -1222,7 +1289,7 @@
       </c>
       <c r="AH3" s="15"/>
     </row>
-    <row r="4" spans="1:34" ht="38.25">
+    <row ht="38.25" r="4" spans="1:34">
       <c r="A4" s="13" t="s">
         <v>10</v>
       </c>
@@ -1312,7 +1379,7 @@
       <c r="AG4" s="16"/>
       <c r="AH4" s="15"/>
     </row>
-    <row r="5" spans="1:34" ht="51">
+    <row ht="51" r="5" spans="1:34">
       <c r="A5" s="13" t="s">
         <v>10</v>
       </c>
@@ -1406,7 +1473,7 @@
       </c>
       <c r="AH5" s="15"/>
     </row>
-    <row r="6" spans="1:34" ht="38.25">
+    <row ht="38.25" r="6" spans="1:34">
       <c r="A6" s="13" t="s">
         <v>10</v>
       </c>
@@ -1502,7 +1569,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="7" spans="1:34" ht="38.25">
+    <row ht="38.25" r="7" spans="1:34">
       <c r="A7" s="13" t="s">
         <v>10</v>
       </c>
@@ -1594,7 +1661,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:34" ht="38.25">
+    <row ht="38.25" r="8" spans="1:34">
       <c r="A8" s="13" t="s">
         <v>10</v>
       </c>
@@ -1688,7 +1755,7 @@
       </c>
       <c r="AH8" s="15"/>
     </row>
-    <row r="9" spans="1:34" ht="51">
+    <row ht="51" r="9" spans="1:34">
       <c r="A9" s="13" t="s">
         <v>10</v>
       </c>
@@ -1782,7 +1849,7 @@
       </c>
       <c r="AH9" s="15"/>
     </row>
-    <row r="10" spans="1:34" s="9" customFormat="1" ht="89.25">
+    <row customFormat="1" ht="89.25" r="10" s="9" spans="1:34">
       <c r="A10" s="13" t="s">
         <v>10</v>
       </c>
@@ -1911,14 +1978,14 @@
       <c r="AH11" s="15"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:W5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
@@ -1926,29 +1993,29 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.5703125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.28515625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.42578125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.28515625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="21.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="8.42578125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="7" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="11" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="7" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="7.42578125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="17.28515625" style="3" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="11.28515625" style="3" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="7.42578125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="7.28515625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="10" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="12.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="9.42578125" style="3" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="18.140625" style="4" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="10.42578125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="18.140625" style="3" customWidth="1" collapsed="1"/>
-    <col min="23" max="16384" width="9.140625" style="8" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="19.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="3" width="14.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="3" width="11.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="3" width="8.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="3" width="17.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="3" width="21.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="3" width="8.42578125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="3" width="7.0" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="3" width="11.0" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="3" width="7.0" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="3" width="7.42578125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="3" width="17.28515625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="3" width="11.28515625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="3" width="7.42578125" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="3" width="7.28515625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" style="3" width="10.0" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="3" width="12.7109375" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" style="3" width="9.42578125" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" style="4" width="18.140625" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" style="3" width="10.42578125" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" style="3" width="18.140625" collapsed="true"/>
+    <col min="23" max="16384" style="8" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
@@ -2214,7 +2281,7 @@
       <c r="V5" s="6"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>